<commit_message>
Fixed bug in PDF-reading of national tests due to FHI changing structure
</commit_message>
<xml_diff>
--- a/data/03_covid_tests/national_tests.xlsx
+++ b/data/03_covid_tests/national_tests.xlsx
@@ -385,6 +385,9 @@
       <c r="A2" s="2">
         <v>43940</v>
       </c>
+      <c r="B2">
+        <v>2498</v>
+      </c>
       <c r="C2">
         <v>142166</v>
       </c>
@@ -392,6 +395,9 @@
     <row r="3">
       <c r="A3" s="2">
         <v>43939</v>
+      </c>
+      <c r="B3">
+        <v>3432</v>
       </c>
       <c r="C3">
         <v>139668</v>

</xml_diff>